<commit_message>
Add hypertension and diabetes clinic
</commit_message>
<xml_diff>
--- a/doctors.xlsx
+++ b/doctors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t xml:space="preserve">Worker</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">Skill Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can_hypertension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can_diabetes</t>
   </si>
   <si>
     <t xml:space="preserve">Mon Start</t>
@@ -246,13 +252,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.17"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -306,24 +316,31 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>0</v>
@@ -359,26 +376,34 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>19</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>12</v>
@@ -387,53 +412,61 @@
         <v>19</v>
       </c>
       <c r="H3" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J3" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N3" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O3" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="P3" s="1" t="n">
         <v>12</v>
       </c>
       <c r="Q3" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S3" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <f aca="false">RANDBETWEEN(1,3)</f>
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
-      </c>
       <c r="D4" s="1" t="n">
-        <v>5</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>15</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>5</v>
@@ -442,163 +475,187 @@
         <v>15</v>
       </c>
       <c r="H4" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J4" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K4" s="1" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L4" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N4" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Q4" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S4" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>15</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>24</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J5" s="1" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K5" s="1" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N5" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O5" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P5" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="S5" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>8</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>20</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J6" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K6" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L6" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N6" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O6" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P6" s="1" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S6" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="n">
+        <f aca="false">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>0</v>
@@ -634,26 +691,34 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
         <v>1</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>19</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>12</v>
@@ -662,53 +727,61 @@
         <v>19</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J8" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K8" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L8" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="M8" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N8" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O8" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="P8" s="1" t="n">
         <v>12</v>
       </c>
       <c r="Q8" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S8" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>5</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>15</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>5</v>
@@ -717,163 +790,187 @@
         <v>15</v>
       </c>
       <c r="H9" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J9" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K9" s="1" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L9" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N9" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="O9" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Q9" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S9" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>15</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>20</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="n">
         <v>20</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J10" s="1" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K10" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M10" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="L10" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="M10" s="1" t="n">
-        <v>19</v>
-      </c>
       <c r="N10" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O10" s="1" t="n">
         <v>19</v>
       </c>
       <c r="P10" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q10" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="S10" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>8</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>20</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H11" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J11" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K11" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L11" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N11" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O11" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="Q11" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S11" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>0</v>
@@ -894,96 +991,112 @@
         <v>12</v>
       </c>
       <c r="L12" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="N12" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O12" s="1" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="P12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
         <v>3</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>8</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>19</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F13" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G13" s="1" t="n">
         <v>19</v>
       </c>
       <c r="H13" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J13" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L13" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N13" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O13" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="P13" s="1" t="n">
         <v>12</v>
       </c>
       <c r="Q13" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S13" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>5</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>15</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="n">
         <v>5</v>
@@ -992,163 +1105,187 @@
         <v>15</v>
       </c>
       <c r="H14" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J14" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L14" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N14" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="O14" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Q14" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S14" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>15</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>24</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F15" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G15" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H15" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J15" s="1" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L15" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N15" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O15" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="S15" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>8</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>20</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F16" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G16" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J16" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="L16" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="K16" s="1" t="n">
+      <c r="M16" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="L16" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="M16" s="1" t="n">
-        <v>20</v>
-      </c>
       <c r="N16" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="P16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="O16" s="1" t="n">
+      <c r="Q16" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="P16" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q16" s="1" t="n">
+      <c r="R16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S16" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
         <v>1</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>0</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F17" s="1" t="n">
         <v>0</v>
@@ -1184,26 +1321,34 @@
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="R17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>19</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F18" s="1" t="n">
         <v>12</v>
@@ -1212,7 +1357,7 @@
         <v>19</v>
       </c>
       <c r="H18" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I18" s="1" t="n">
         <v>19</v>
@@ -1221,44 +1366,52 @@
         <v>8</v>
       </c>
       <c r="K18" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L18" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="N18" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O18" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Q18" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="R18" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S18" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>5</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>15</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>5</v>
@@ -1267,163 +1420,187 @@
         <v>15</v>
       </c>
       <c r="H19" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J19" s="1" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K19" s="1" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L19" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="M19" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N19" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="O19" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="Q19" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R19" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S19" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>11</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>20</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F20" s="1" t="n">
         <v>11</v>
       </c>
       <c r="G20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="I20" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="H20" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>24</v>
-      </c>
       <c r="J20" s="1" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="K20" s="1" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="L20" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="N20" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O20" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P20" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q20" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="S20" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C21" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
         <v>2</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>8</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>20</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G21" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H21" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J21" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L21" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="M21" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N21" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O21" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P21" s="1" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="Q21" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R21" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S21" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" s="1" t="n">
+        <f aca="false">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>0</v>
@@ -1459,26 +1636,34 @@
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="R22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>12</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>19</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="F23" s="1" t="n">
         <v>12</v>
@@ -1487,25 +1672,25 @@
         <v>19</v>
       </c>
       <c r="H23" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J23" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K23" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L23" s="1" t="n">
         <v>8</v>
       </c>
       <c r="M23" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N23" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O23" s="1" t="n">
         <v>19</v>
@@ -1514,171 +1699,201 @@
         <v>12</v>
       </c>
       <c r="Q23" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="R23" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="S23" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B24" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1" t="n">
+        <f aca="false">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c r="E24" s="1" t="n">
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G24" s="1" t="n">
+      <c r="H24" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I24" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="H24" s="1" t="n">
+      <c r="J24" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="I24" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="J24" s="1" t="n">
-        <v>15</v>
-      </c>
       <c r="K24" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="M24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="L24" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="M24" s="1" t="n">
-        <v>20</v>
-      </c>
       <c r="N24" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="P24" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="O24" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="P24" s="1" t="n">
-        <v>8</v>
-      </c>
       <c r="Q24" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="R24" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S24" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C25" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>15</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>24</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G25" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="H25" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="J25" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K25" s="1" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L25" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="M25" s="1" t="n">
         <v>19</v>
       </c>
       <c r="N25" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="O25" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P25" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q25" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="R25" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="S25" s="1" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,50)</f>
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1" t="n">
         <f aca="false">RANDBETWEEN(1,3)</f>
         <v>1</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>8</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="E26" s="1" t="n">
-        <v>20</v>
+        <f aca="false">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="F26" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G26" s="1" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H26" s="1" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J26" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K26" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L26" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="M26" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N26" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="O26" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="P26" s="1" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="Q26" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R26" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="S26" s="1" t="n">
         <v>24</v>
       </c>
     </row>

</xml_diff>